<commit_message>
Actualización solicitud gráfica CN_06_02_CO_REC_10
Actualización solicitud gráfica CN_06_02_CO_REC_10
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/SolicitudGrafica_CN_06_02_CO_REC10.xlsx
+++ b/fuentes/contenidos/grado06/guion02/SolicitudGrafica_CN_06_02_CO_REC10.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="197">
   <si>
     <t>Fecha:</t>
   </si>
@@ -615,9 +615,6 @@
   </si>
   <si>
     <t>Neuronas</t>
-  </si>
-  <si>
-    <t>Guarda foto girada 90°</t>
   </si>
   <si>
     <t>División celular con cromosomas</t>
@@ -1783,6 +1780,341 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>11207</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1725705</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16371795" y="2185147"/>
+          <a:ext cx="2253375" cy="1692087"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>56030</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>56030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>33618</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1725706</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16416618" y="4022912"/>
+          <a:ext cx="2229971" cy="1669676"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2229971</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1512894</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagen 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16371794" y="5793442"/>
+          <a:ext cx="2218765" cy="1479276"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161134</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2192343</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1650801</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagen 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16509498" y="7429500"/>
+          <a:ext cx="2031209" cy="1633483"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>99391</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>11991</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2219738</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1587592</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagen 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16474108" y="9064882"/>
+          <a:ext cx="2120347" cy="1575601"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>136737</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2234044</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1645227</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Imagen 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16485101" y="10711218"/>
+          <a:ext cx="2097307" cy="1619327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
@@ -2496,9 +2828,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I14" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2786,7 +3117,7 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="11" customFormat="1" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
@@ -2829,7 +3160,7 @@
         <v>M12D</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="11" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="str">
         <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
@@ -2872,7 +3203,7 @@
         <v>M101</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG03</v>
@@ -2915,7 +3246,7 @@
         <v>Diaporama F1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG04</v>
@@ -2958,7 +3289,7 @@
         <v>F4</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="11" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG05</v>
@@ -3001,7 +3332,7 @@
         <v>F6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG06</v>
@@ -3036,11 +3367,9 @@
         <v/>
       </c>
       <c r="J15" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="K15" s="66" t="s">
         <v>196</v>
       </c>
+      <c r="K15" s="66"/>
       <c r="O15" s="2" t="str">
         <f>'Definición técnica de imagenes'!A24</f>
         <v>F6B</v>
@@ -6011,6 +6340,7 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>